<commit_message>
updated scripts and datasheet
</commit_message>
<xml_diff>
--- a/TN5250/artifact/data/TN5250.data.xlsx
+++ b/TN5250/artifact/data/TN5250.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
   </si>
@@ -257,6 +257,18 @@
   </si>
   <si>
     <t>SarathN</t>
+  </si>
+  <si>
+    <t>stringStart</t>
+  </si>
+  <si>
+    <t>....+....1....+....2....+....3....+....4....+....5....+....6....+....7..</t>
+  </si>
+  <si>
+    <t>stringEnd</t>
+  </si>
+  <si>
+    <t>****** ********  End of report  ********</t>
   </si>
 </sst>
 </file>
@@ -1365,8 +1377,8 @@
   <sheetPr/>
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="1"/>
@@ -1649,11 +1661,21 @@
         <v>62</v>
       </c>
     </row>
-    <row r="35" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A35" s="4"/>
-    </row>
-    <row r="36" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A36" s="4"/>
+    <row r="35" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A35" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A36" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="37" ht="23.1" customHeight="1" spans="1:1">
       <c r="A37" s="4"/>

</xml_diff>